<commit_message>
variabler på plass, ikke tatt så mye i bruk, mest i processpr _update_all_metrics
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251112-tett6roof/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251112-tett6roof/meta.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DL44"/>
+  <dimension ref="A1:DF44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,57 +869,57 @@
       </c>
       <c r="CL1" t="inlineStr">
         <is>
-          <t>Wavefrequency (given)</t>
+          <t>Waveperiod</t>
         </is>
       </c>
       <c r="CM1" t="inlineStr">
         <is>
-          <t>Waveperiod (given)</t>
+          <t>Wavenumber</t>
         </is>
       </c>
       <c r="CN1" t="inlineStr">
         <is>
-          <t>Wavenumber (given)</t>
+          <t>Wavelength</t>
         </is>
       </c>
       <c r="CO1" t="inlineStr">
         <is>
-          <t>Wavelength (given)</t>
+          <t>kL</t>
         </is>
       </c>
       <c r="CP1" t="inlineStr">
         <is>
-          <t>kL (given)</t>
+          <t>ak</t>
         </is>
       </c>
       <c r="CQ1" t="inlineStr">
         <is>
-          <t>ak (given)</t>
+          <t>kH</t>
         </is>
       </c>
       <c r="CR1" t="inlineStr">
         <is>
-          <t>kH (given)</t>
+          <t>tanh(kH)</t>
         </is>
       </c>
       <c r="CS1" t="inlineStr">
         <is>
-          <t>tanh(kH) (given)</t>
+          <t>Celerity</t>
         </is>
       </c>
       <c r="CT1" t="inlineStr">
         <is>
-          <t>Celerity (given)</t>
+          <t>Significant Wave Height Hs</t>
         </is>
       </c>
       <c r="CU1" t="inlineStr">
         <is>
-          <t>Significant Wave Height Hs (given)</t>
+          <t>Significant Wave Height Hm0</t>
         </is>
       </c>
       <c r="CV1" t="inlineStr">
         <is>
-          <t>Significant Wave Height Hm0 (given)</t>
+          <t>Reynoldsnumber (Water)</t>
         </is>
       </c>
       <c r="CW1" t="inlineStr">
@@ -929,77 +929,47 @@
       </c>
       <c r="CX1" t="inlineStr">
         <is>
+          <t>Reynoldsnumber (Wind)</t>
+        </is>
+      </c>
+      <c r="CY1" t="inlineStr">
+        <is>
           <t>P2/P1 (FFT)</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>P3/P2 (FFT)</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>P4/P3 (FFT)</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>PROCESSED_folder</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>Probe 1 Frequency (FFT)</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>Probe 2 Frequency (FFT)</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>Probe 3 Frequency (FFT)</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>Probe 4 Frequency (FFT)</t>
-        </is>
-      </c>
-      <c r="DF1" t="inlineStr">
-        <is>
-          <t>Wavenumber</t>
-        </is>
-      </c>
-      <c r="DG1" t="inlineStr">
-        <is>
-          <t>Wavelength</t>
-        </is>
-      </c>
-      <c r="DH1" t="inlineStr">
-        <is>
-          <t>kL</t>
-        </is>
-      </c>
-      <c r="DI1" t="inlineStr">
-        <is>
-          <t>ak</t>
-        </is>
-      </c>
-      <c r="DJ1" t="inlineStr">
-        <is>
-          <t>kH</t>
-        </is>
-      </c>
-      <c r="DK1" t="inlineStr">
-        <is>
-          <t>tanh(kH)</t>
-        </is>
-      </c>
-      <c r="DL1" t="inlineStr">
-        <is>
-          <t>Celerity</t>
         </is>
       </c>
     </row>
@@ -1260,35 +1230,45 @@
       <c r="CJ2" t="inlineStr"/>
       <c r="CK2" t="inlineStr"/>
       <c r="CL2" t="inlineStr"/>
-      <c r="CM2" t="inlineStr"/>
-      <c r="CN2" t="inlineStr"/>
+      <c r="CM2" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO2" t="inlineStr"/>
-      <c r="CP2" t="inlineStr"/>
-      <c r="CQ2" t="inlineStr"/>
-      <c r="CR2" t="inlineStr"/>
-      <c r="CS2" t="inlineStr"/>
+      <c r="CP2" t="n">
+        <v>0.166242017140429</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT2" t="inlineStr"/>
       <c r="CU2" t="inlineStr"/>
       <c r="CV2" t="inlineStr"/>
       <c r="CW2" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX2" t="n">
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="n">
         <v>1.011336447675711</v>
       </c>
-      <c r="CY2" t="n">
+      <c r="CZ2" t="n">
         <v>0.9501802213991354</v>
       </c>
-      <c r="CZ2" t="n">
+      <c r="DA2" t="n">
         <v>1.048557063364884</v>
       </c>
-      <c r="DA2" t="inlineStr">
+      <c r="DB2" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB2" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC2" t="n">
         <v>1.299826689774697</v>
@@ -1300,23 +1280,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF2" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH2" t="inlineStr"/>
-      <c r="DI2" t="n">
-        <v>0.166242017140429</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="3">
@@ -1584,35 +1548,47 @@
       <c r="CJ3" t="inlineStr"/>
       <c r="CK3" t="inlineStr"/>
       <c r="CL3" t="inlineStr"/>
-      <c r="CM3" t="inlineStr"/>
-      <c r="CN3" t="inlineStr"/>
-      <c r="CO3" t="inlineStr"/>
-      <c r="CP3" t="inlineStr"/>
-      <c r="CQ3" t="inlineStr"/>
-      <c r="CR3" t="inlineStr"/>
-      <c r="CS3" t="inlineStr"/>
+      <c r="CM3" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>0.02910602518531768</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT3" t="inlineStr"/>
       <c r="CU3" t="inlineStr"/>
       <c r="CV3" t="inlineStr"/>
       <c r="CW3" t="n">
         <v>0</v>
       </c>
-      <c r="CX3" t="n">
+      <c r="CX3" t="inlineStr"/>
+      <c r="CY3" t="n">
         <v>1.044162970336802</v>
       </c>
-      <c r="CY3" t="n">
+      <c r="CZ3" t="n">
         <v>0.9696157709281857</v>
       </c>
-      <c r="CZ3" t="n">
+      <c r="DA3" t="n">
         <v>1.003088565524012</v>
       </c>
-      <c r="DA3" t="inlineStr">
+      <c r="DB3" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB3" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC3" t="n">
         <v>0.6499837504062399</v>
@@ -1624,25 +1600,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF3" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG3" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH3" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI3" t="n">
-        <v>0.02910602518531768</v>
-      </c>
-      <c r="DJ3" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK3" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL3" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="4">
@@ -1818,22 +1776,16 @@
       <c r="CX4" t="inlineStr"/>
       <c r="CY4" t="inlineStr"/>
       <c r="CZ4" t="inlineStr"/>
-      <c r="DA4" t="inlineStr">
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB4" t="inlineStr"/>
       <c r="DC4" t="inlineStr"/>
       <c r="DD4" t="inlineStr"/>
       <c r="DE4" t="inlineStr"/>
       <c r="DF4" t="inlineStr"/>
-      <c r="DG4" t="inlineStr"/>
-      <c r="DH4" t="inlineStr"/>
-      <c r="DI4" t="inlineStr"/>
-      <c r="DJ4" t="inlineStr"/>
-      <c r="DK4" t="inlineStr"/>
-      <c r="DL4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2092,63 +2044,57 @@
       <c r="CJ5" t="inlineStr"/>
       <c r="CK5" t="inlineStr"/>
       <c r="CL5" t="inlineStr"/>
-      <c r="CM5" t="inlineStr"/>
-      <c r="CN5" t="inlineStr"/>
+      <c r="CM5" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO5" t="inlineStr"/>
-      <c r="CP5" t="inlineStr"/>
-      <c r="CQ5" t="inlineStr"/>
-      <c r="CR5" t="inlineStr"/>
-      <c r="CS5" t="inlineStr"/>
+      <c r="CP5" t="n">
+        <v>0.06047013373816879</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT5" t="inlineStr"/>
       <c r="CU5" t="inlineStr"/>
       <c r="CV5" t="inlineStr"/>
       <c r="CW5" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX5" t="n">
+      <c r="CX5" t="inlineStr"/>
+      <c r="CY5" t="n">
         <v>1.012872225174823</v>
       </c>
-      <c r="CY5" t="n">
+      <c r="CZ5" t="n">
         <v>1.014358044141053</v>
       </c>
-      <c r="CZ5" t="n">
+      <c r="DA5" t="n">
         <v>1.036939680368307</v>
       </c>
-      <c r="DA5" t="inlineStr">
+      <c r="DB5" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB5" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC5" t="n">
         <v>1.299826689774697</v>
       </c>
       <c r="DD5" t="n">
+        <v>1.299826689774697</v>
+      </c>
+      <c r="DE5" t="n">
         <v>1.300108342361864</v>
       </c>
-      <c r="DE5" t="n">
+      <c r="DF5" t="n">
         <v>1.299826689774697</v>
-      </c>
-      <c r="DF5" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG5" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH5" t="inlineStr"/>
-      <c r="DI5" t="n">
-        <v>0.06047013373816879</v>
-      </c>
-      <c r="DJ5" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK5" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL5" t="n">
-        <v>1.19970570478913</v>
       </c>
     </row>
     <row r="6">
@@ -2416,35 +2362,47 @@
       <c r="CJ6" t="inlineStr"/>
       <c r="CK6" t="inlineStr"/>
       <c r="CL6" t="inlineStr"/>
-      <c r="CM6" t="inlineStr"/>
-      <c r="CN6" t="inlineStr"/>
-      <c r="CO6" t="inlineStr"/>
-      <c r="CP6" t="inlineStr"/>
-      <c r="CQ6" t="inlineStr"/>
-      <c r="CR6" t="inlineStr"/>
-      <c r="CS6" t="inlineStr"/>
+      <c r="CM6" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>0.009814703318385815</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT6" t="inlineStr"/>
       <c r="CU6" t="inlineStr"/>
       <c r="CV6" t="inlineStr"/>
       <c r="CW6" t="n">
         <v>0</v>
       </c>
-      <c r="CX6" t="n">
+      <c r="CX6" t="inlineStr"/>
+      <c r="CY6" t="n">
         <v>1.053504371600242</v>
       </c>
-      <c r="CY6" t="n">
+      <c r="CZ6" t="n">
         <v>0.9715811770956726</v>
       </c>
-      <c r="CZ6" t="n">
+      <c r="DA6" t="n">
         <v>1.005264131057575</v>
       </c>
-      <c r="DA6" t="inlineStr">
+      <c r="DB6" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB6" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC6" t="n">
         <v>0.6499837504062399</v>
@@ -2456,25 +2414,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF6" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG6" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH6" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI6" t="n">
-        <v>0.009814703318385815</v>
-      </c>
-      <c r="DJ6" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK6" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL6" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="7">
@@ -2734,63 +2674,57 @@
       <c r="CJ7" t="inlineStr"/>
       <c r="CK7" t="inlineStr"/>
       <c r="CL7" t="inlineStr"/>
-      <c r="CM7" t="inlineStr"/>
-      <c r="CN7" t="inlineStr"/>
+      <c r="CM7" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO7" t="inlineStr"/>
-      <c r="CP7" t="inlineStr"/>
-      <c r="CQ7" t="inlineStr"/>
-      <c r="CR7" t="inlineStr"/>
-      <c r="CS7" t="inlineStr"/>
+      <c r="CP7" t="n">
+        <v>0.022200899886161</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR7" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS7" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT7" t="inlineStr"/>
       <c r="CU7" t="inlineStr"/>
       <c r="CV7" t="inlineStr"/>
       <c r="CW7" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX7" t="n">
+      <c r="CX7" t="inlineStr"/>
+      <c r="CY7" t="n">
         <v>1.03709056210268</v>
       </c>
-      <c r="CY7" t="n">
+      <c r="CZ7" t="n">
         <v>0.9673806146154074</v>
       </c>
-      <c r="CZ7" t="n">
+      <c r="DA7" t="n">
         <v>1.018331230674218</v>
       </c>
-      <c r="DA7" t="inlineStr">
+      <c r="DB7" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB7" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC7" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DD7" t="n">
+        <v>0.6499837504062399</v>
+      </c>
+      <c r="DE7" t="n">
         <v>0.6500541711809318</v>
       </c>
-      <c r="DE7" t="n">
+      <c r="DF7" t="n">
         <v>0.6499837504062399</v>
-      </c>
-      <c r="DF7" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG7" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH7" t="inlineStr"/>
-      <c r="DI7" t="n">
-        <v>0.022200899886161</v>
-      </c>
-      <c r="DJ7" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK7" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL7" t="n">
-        <v>1.993203138117973</v>
       </c>
     </row>
     <row r="8">
@@ -3058,35 +2992,47 @@
       <c r="CJ8" t="inlineStr"/>
       <c r="CK8" t="inlineStr"/>
       <c r="CL8" t="inlineStr"/>
-      <c r="CM8" t="inlineStr"/>
-      <c r="CN8" t="inlineStr"/>
-      <c r="CO8" t="inlineStr"/>
-      <c r="CP8" t="inlineStr"/>
-      <c r="CQ8" t="inlineStr"/>
-      <c r="CR8" t="inlineStr"/>
-      <c r="CS8" t="inlineStr"/>
+      <c r="CM8" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO8" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP8" t="n">
+        <v>0.1132467146496721</v>
+      </c>
+      <c r="CQ8" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR8" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS8" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT8" t="inlineStr"/>
       <c r="CU8" t="inlineStr"/>
       <c r="CV8" t="inlineStr"/>
       <c r="CW8" t="n">
         <v>0</v>
       </c>
-      <c r="CX8" t="n">
+      <c r="CX8" t="inlineStr"/>
+      <c r="CY8" t="n">
         <v>1.000232244319276</v>
       </c>
-      <c r="CY8" t="n">
+      <c r="CZ8" t="n">
         <v>0.7097443096061512</v>
       </c>
-      <c r="CZ8" t="n">
+      <c r="DA8" t="n">
         <v>1.027726942846914</v>
       </c>
-      <c r="DA8" t="inlineStr">
+      <c r="DB8" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB8" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC8" t="n">
         <v>1.299826689774697</v>
@@ -3098,25 +3044,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF8" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG8" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH8" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI8" t="n">
-        <v>0.1132467146496721</v>
-      </c>
-      <c r="DJ8" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK8" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL8" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="9">
@@ -3376,63 +3304,57 @@
       <c r="CJ9" t="inlineStr"/>
       <c r="CK9" t="inlineStr"/>
       <c r="CL9" t="inlineStr"/>
-      <c r="CM9" t="inlineStr"/>
-      <c r="CN9" t="inlineStr"/>
+      <c r="CM9" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO9" t="inlineStr"/>
-      <c r="CP9" t="inlineStr"/>
-      <c r="CQ9" t="inlineStr"/>
-      <c r="CR9" t="inlineStr"/>
-      <c r="CS9" t="inlineStr"/>
+      <c r="CP9" t="n">
+        <v>0.01268330136551323</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR9" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS9" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT9" t="inlineStr"/>
       <c r="CU9" t="inlineStr"/>
       <c r="CV9" t="inlineStr"/>
       <c r="CW9" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX9" t="n">
+      <c r="CX9" t="inlineStr"/>
+      <c r="CY9" t="n">
         <v>1.019573777652404</v>
       </c>
-      <c r="CY9" t="n">
+      <c r="CZ9" t="n">
         <v>1.002510224035701</v>
       </c>
-      <c r="CZ9" t="n">
+      <c r="DA9" t="n">
         <v>0.9787999311488548</v>
       </c>
-      <c r="DA9" t="inlineStr">
+      <c r="DB9" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB9" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC9" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DD9" t="n">
-        <v>0.6500541711809318</v>
+        <v>0.6499837504062399</v>
       </c>
       <c r="DE9" t="n">
         <v>0.6500541711809318</v>
       </c>
       <c r="DF9" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG9" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH9" t="inlineStr"/>
-      <c r="DI9" t="n">
-        <v>0.01268330136551323</v>
-      </c>
-      <c r="DJ9" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK9" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL9" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6500541711809318</v>
       </c>
     </row>
     <row r="10">
@@ -3700,35 +3622,47 @@
       <c r="CJ10" t="inlineStr"/>
       <c r="CK10" t="inlineStr"/>
       <c r="CL10" t="inlineStr"/>
-      <c r="CM10" t="inlineStr"/>
-      <c r="CN10" t="inlineStr"/>
-      <c r="CO10" t="inlineStr"/>
-      <c r="CP10" t="inlineStr"/>
-      <c r="CQ10" t="inlineStr"/>
-      <c r="CR10" t="inlineStr"/>
-      <c r="CS10" t="inlineStr"/>
+      <c r="CM10" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO10" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP10" t="n">
+        <v>0.05562506778217258</v>
+      </c>
+      <c r="CQ10" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR10" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS10" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT10" t="inlineStr"/>
       <c r="CU10" t="inlineStr"/>
       <c r="CV10" t="inlineStr"/>
       <c r="CW10" t="n">
         <v>0</v>
       </c>
-      <c r="CX10" t="n">
+      <c r="CX10" t="inlineStr"/>
+      <c r="CY10" t="n">
         <v>0.9786678979529024</v>
       </c>
-      <c r="CY10" t="n">
+      <c r="CZ10" t="n">
         <v>0.6766989732725671</v>
       </c>
-      <c r="CZ10" t="n">
+      <c r="DA10" t="n">
         <v>1.029915392881313</v>
       </c>
-      <c r="DA10" t="inlineStr">
+      <c r="DB10" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB10" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC10" t="n">
         <v>1.299826689774697</v>
@@ -3740,25 +3674,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF10" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG10" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH10" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI10" t="n">
-        <v>0.05562506778217258</v>
-      </c>
-      <c r="DJ10" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK10" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL10" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="11">
@@ -4026,35 +3942,47 @@
       <c r="CJ11" t="inlineStr"/>
       <c r="CK11" t="inlineStr"/>
       <c r="CL11" t="inlineStr"/>
-      <c r="CM11" t="inlineStr"/>
-      <c r="CN11" t="inlineStr"/>
-      <c r="CO11" t="inlineStr"/>
-      <c r="CP11" t="inlineStr"/>
-      <c r="CQ11" t="inlineStr"/>
-      <c r="CR11" t="inlineStr"/>
-      <c r="CS11" t="inlineStr"/>
+      <c r="CM11" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO11" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP11" t="n">
+        <v>0.05443358836211374</v>
+      </c>
+      <c r="CQ11" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR11" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS11" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT11" t="inlineStr"/>
       <c r="CU11" t="inlineStr"/>
       <c r="CV11" t="inlineStr"/>
       <c r="CW11" t="n">
         <v>0</v>
       </c>
-      <c r="CX11" t="n">
+      <c r="CX11" t="inlineStr"/>
+      <c r="CY11" t="n">
         <v>0.9238849845864656</v>
       </c>
-      <c r="CY11" t="n">
+      <c r="CZ11" t="n">
         <v>0.7014382994437879</v>
       </c>
-      <c r="CZ11" t="n">
+      <c r="DA11" t="n">
         <v>1.035096802498275</v>
       </c>
-      <c r="DA11" t="inlineStr">
+      <c r="DB11" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB11" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC11" t="n">
         <v>1.299826689774697</v>
@@ -4066,25 +3994,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF11" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG11" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH11" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI11" t="n">
-        <v>0.05443358836211374</v>
-      </c>
-      <c r="DJ11" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK11" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL11" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="12">
@@ -4344,63 +4254,57 @@
       <c r="CJ12" t="inlineStr"/>
       <c r="CK12" t="inlineStr"/>
       <c r="CL12" t="inlineStr"/>
-      <c r="CM12" t="inlineStr"/>
-      <c r="CN12" t="inlineStr"/>
+      <c r="CM12" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN12" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO12" t="inlineStr"/>
-      <c r="CP12" t="inlineStr"/>
-      <c r="CQ12" t="inlineStr"/>
-      <c r="CR12" t="inlineStr"/>
-      <c r="CS12" t="inlineStr"/>
+      <c r="CP12" t="n">
+        <v>0.01277550630274236</v>
+      </c>
+      <c r="CQ12" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR12" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS12" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT12" t="inlineStr"/>
       <c r="CU12" t="inlineStr"/>
       <c r="CV12" t="inlineStr"/>
       <c r="CW12" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX12" t="n">
+      <c r="CX12" t="inlineStr"/>
+      <c r="CY12" t="n">
         <v>1.033102191917685</v>
       </c>
-      <c r="CY12" t="n">
+      <c r="CZ12" t="n">
         <v>1.004577508931341</v>
       </c>
-      <c r="CZ12" t="n">
+      <c r="DA12" t="n">
         <v>0.9921151426193191</v>
       </c>
-      <c r="DA12" t="inlineStr">
+      <c r="DB12" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB12" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC12" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DD12" t="n">
-        <v>0.6500541711809318</v>
+        <v>0.6499837504062399</v>
       </c>
       <c r="DE12" t="n">
         <v>0.6500541711809318</v>
       </c>
       <c r="DF12" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG12" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH12" t="inlineStr"/>
-      <c r="DI12" t="n">
-        <v>0.01277550630274236</v>
-      </c>
-      <c r="DJ12" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK12" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL12" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6500541711809318</v>
       </c>
     </row>
     <row r="13">
@@ -4660,35 +4564,45 @@
       <c r="CJ13" t="inlineStr"/>
       <c r="CK13" t="inlineStr"/>
       <c r="CL13" t="inlineStr"/>
-      <c r="CM13" t="inlineStr"/>
-      <c r="CN13" t="inlineStr"/>
+      <c r="CM13" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN13" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO13" t="inlineStr"/>
-      <c r="CP13" t="inlineStr"/>
-      <c r="CQ13" t="inlineStr"/>
-      <c r="CR13" t="inlineStr"/>
-      <c r="CS13" t="inlineStr"/>
+      <c r="CP13" t="n">
+        <v>0.1149607429010995</v>
+      </c>
+      <c r="CQ13" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR13" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS13" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT13" t="inlineStr"/>
       <c r="CU13" t="inlineStr"/>
       <c r="CV13" t="inlineStr"/>
       <c r="CW13" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX13" t="n">
+      <c r="CX13" t="inlineStr"/>
+      <c r="CY13" t="n">
         <v>1.01355468652777</v>
       </c>
-      <c r="CY13" t="n">
+      <c r="CZ13" t="n">
         <v>1.024205767586054</v>
       </c>
-      <c r="CZ13" t="n">
+      <c r="DA13" t="n">
         <v>0.9323278848873658</v>
       </c>
-      <c r="DA13" t="inlineStr">
+      <c r="DB13" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB13" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC13" t="n">
         <v>1.299826689774697</v>
@@ -4700,23 +4614,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF13" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG13" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH13" t="inlineStr"/>
-      <c r="DI13" t="n">
-        <v>0.1149607429010995</v>
-      </c>
-      <c r="DJ13" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK13" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL13" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="14">
@@ -4984,35 +4882,47 @@
       <c r="CJ14" t="inlineStr"/>
       <c r="CK14" t="inlineStr"/>
       <c r="CL14" t="inlineStr"/>
-      <c r="CM14" t="inlineStr"/>
-      <c r="CN14" t="inlineStr"/>
-      <c r="CO14" t="inlineStr"/>
-      <c r="CP14" t="inlineStr"/>
-      <c r="CQ14" t="inlineStr"/>
-      <c r="CR14" t="inlineStr"/>
-      <c r="CS14" t="inlineStr"/>
+      <c r="CM14" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN14" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO14" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP14" t="n">
+        <v>0.01981381651122995</v>
+      </c>
+      <c r="CQ14" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR14" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS14" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT14" t="inlineStr"/>
       <c r="CU14" t="inlineStr"/>
       <c r="CV14" t="inlineStr"/>
       <c r="CW14" t="n">
         <v>0</v>
       </c>
-      <c r="CX14" t="n">
+      <c r="CX14" t="inlineStr"/>
+      <c r="CY14" t="n">
         <v>1.049993344681407</v>
       </c>
-      <c r="CY14" t="n">
+      <c r="CZ14" t="n">
         <v>0.9698762960193082</v>
       </c>
-      <c r="CZ14" t="n">
+      <c r="DA14" t="n">
         <v>1.000801970199081</v>
       </c>
-      <c r="DA14" t="inlineStr">
+      <c r="DB14" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB14" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC14" t="n">
         <v>0.6499837504062399</v>
@@ -5024,25 +4934,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF14" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG14" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH14" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI14" t="n">
-        <v>0.01981381651122995</v>
-      </c>
-      <c r="DJ14" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK14" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL14" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="15">
@@ -5310,35 +5202,47 @@
       <c r="CJ15" t="inlineStr"/>
       <c r="CK15" t="inlineStr"/>
       <c r="CL15" t="inlineStr"/>
-      <c r="CM15" t="inlineStr"/>
-      <c r="CN15" t="inlineStr"/>
-      <c r="CO15" t="inlineStr"/>
-      <c r="CP15" t="inlineStr"/>
-      <c r="CQ15" t="inlineStr"/>
-      <c r="CR15" t="inlineStr"/>
-      <c r="CS15" t="inlineStr"/>
+      <c r="CM15" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN15" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO15" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP15" t="n">
+        <v>0.05678250493308674</v>
+      </c>
+      <c r="CQ15" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR15" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS15" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT15" t="inlineStr"/>
       <c r="CU15" t="inlineStr"/>
       <c r="CV15" t="inlineStr"/>
       <c r="CW15" t="n">
         <v>0</v>
       </c>
-      <c r="CX15" t="n">
+      <c r="CX15" t="inlineStr"/>
+      <c r="CY15" t="n">
         <v>0.9391983752380851</v>
       </c>
-      <c r="CY15" t="n">
+      <c r="CZ15" t="n">
         <v>0.6687555103856894</v>
       </c>
-      <c r="CZ15" t="n">
+      <c r="DA15" t="n">
         <v>1.035592795403869</v>
       </c>
-      <c r="DA15" t="inlineStr">
+      <c r="DB15" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB15" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC15" t="n">
         <v>1.299826689774697</v>
@@ -5350,25 +5254,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF15" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG15" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH15" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI15" t="n">
-        <v>0.05678250493308674</v>
-      </c>
-      <c r="DJ15" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK15" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL15" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="16">
@@ -5552,22 +5438,16 @@
       <c r="CX16" t="inlineStr"/>
       <c r="CY16" t="inlineStr"/>
       <c r="CZ16" t="inlineStr"/>
-      <c r="DA16" t="inlineStr">
+      <c r="DA16" t="inlineStr"/>
+      <c r="DB16" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB16" t="inlineStr"/>
       <c r="DC16" t="inlineStr"/>
       <c r="DD16" t="inlineStr"/>
       <c r="DE16" t="inlineStr"/>
       <c r="DF16" t="inlineStr"/>
-      <c r="DG16" t="inlineStr"/>
-      <c r="DH16" t="inlineStr"/>
-      <c r="DI16" t="inlineStr"/>
-      <c r="DJ16" t="inlineStr"/>
-      <c r="DK16" t="inlineStr"/>
-      <c r="DL16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -5826,63 +5706,57 @@
       <c r="CJ17" t="inlineStr"/>
       <c r="CK17" t="inlineStr"/>
       <c r="CL17" t="inlineStr"/>
-      <c r="CM17" t="inlineStr"/>
-      <c r="CN17" t="inlineStr"/>
+      <c r="CM17" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN17" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO17" t="inlineStr"/>
-      <c r="CP17" t="inlineStr"/>
-      <c r="CQ17" t="inlineStr"/>
-      <c r="CR17" t="inlineStr"/>
-      <c r="CS17" t="inlineStr"/>
+      <c r="CP17" t="n">
+        <v>0.03127796370671412</v>
+      </c>
+      <c r="CQ17" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR17" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS17" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT17" t="inlineStr"/>
       <c r="CU17" t="inlineStr"/>
       <c r="CV17" t="inlineStr"/>
       <c r="CW17" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX17" t="n">
+      <c r="CX17" t="inlineStr"/>
+      <c r="CY17" t="n">
         <v>1.018839537633315</v>
       </c>
-      <c r="CY17" t="n">
+      <c r="CZ17" t="n">
         <v>0.9830592940078693</v>
       </c>
-      <c r="CZ17" t="n">
+      <c r="DA17" t="n">
         <v>1.005635066148295</v>
       </c>
-      <c r="DA17" t="inlineStr">
+      <c r="DB17" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB17" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC17" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DD17" t="n">
-        <v>0.6500541711809318</v>
+        <v>0.6499837504062399</v>
       </c>
       <c r="DE17" t="n">
         <v>0.6500541711809318</v>
       </c>
       <c r="DF17" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG17" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH17" t="inlineStr"/>
-      <c r="DI17" t="n">
-        <v>0.03127796370671412</v>
-      </c>
-      <c r="DJ17" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK17" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL17" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6500541711809318</v>
       </c>
     </row>
     <row r="18">
@@ -6150,35 +6024,47 @@
       <c r="CJ18" t="inlineStr"/>
       <c r="CK18" t="inlineStr"/>
       <c r="CL18" t="inlineStr"/>
-      <c r="CM18" t="inlineStr"/>
-      <c r="CN18" t="inlineStr"/>
-      <c r="CO18" t="inlineStr"/>
-      <c r="CP18" t="inlineStr"/>
-      <c r="CQ18" t="inlineStr"/>
-      <c r="CR18" t="inlineStr"/>
-      <c r="CS18" t="inlineStr"/>
+      <c r="CM18" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN18" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO18" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP18" t="n">
+        <v>0.16585478632891</v>
+      </c>
+      <c r="CQ18" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR18" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS18" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT18" t="inlineStr"/>
       <c r="CU18" t="inlineStr"/>
       <c r="CV18" t="inlineStr"/>
       <c r="CW18" t="n">
         <v>0</v>
       </c>
-      <c r="CX18" t="n">
+      <c r="CX18" t="inlineStr"/>
+      <c r="CY18" t="n">
         <v>1.022673349972923</v>
       </c>
-      <c r="CY18" t="n">
+      <c r="CZ18" t="n">
         <v>0.7394640719643086</v>
       </c>
-      <c r="CZ18" t="n">
+      <c r="DA18" t="n">
         <v>1.023925402439761</v>
       </c>
-      <c r="DA18" t="inlineStr">
+      <c r="DB18" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB18" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC18" t="n">
         <v>1.299826689774697</v>
@@ -6190,25 +6076,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF18" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG18" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH18" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI18" t="n">
-        <v>0.16585478632891</v>
-      </c>
-      <c r="DJ18" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK18" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL18" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="19">
@@ -6468,63 +6336,57 @@
       <c r="CJ19" t="inlineStr"/>
       <c r="CK19" t="inlineStr"/>
       <c r="CL19" t="inlineStr"/>
-      <c r="CM19" t="inlineStr"/>
-      <c r="CN19" t="inlineStr"/>
+      <c r="CM19" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN19" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO19" t="inlineStr"/>
-      <c r="CP19" t="inlineStr"/>
-      <c r="CQ19" t="inlineStr"/>
-      <c r="CR19" t="inlineStr"/>
-      <c r="CS19" t="inlineStr"/>
+      <c r="CP19" t="n">
+        <v>0.03384945695610326</v>
+      </c>
+      <c r="CQ19" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR19" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS19" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT19" t="inlineStr"/>
       <c r="CU19" t="inlineStr"/>
       <c r="CV19" t="inlineStr"/>
       <c r="CW19" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX19" t="n">
+      <c r="CX19" t="inlineStr"/>
+      <c r="CY19" t="n">
         <v>1.017665842415511</v>
       </c>
-      <c r="CY19" t="n">
+      <c r="CZ19" t="n">
         <v>0.9589852054503312</v>
       </c>
-      <c r="CZ19" t="n">
+      <c r="DA19" t="n">
         <v>1.035713722053874</v>
       </c>
-      <c r="DA19" t="inlineStr">
+      <c r="DB19" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB19" t="n">
+      <c r="DC19" t="n">
         <v>0.6500541711809318</v>
       </c>
-      <c r="DC19" t="n">
+      <c r="DD19" t="n">
         <v>0.6499837504062399</v>
       </c>
-      <c r="DD19" t="n">
+      <c r="DE19" t="n">
         <v>0.6501950585175553</v>
       </c>
-      <c r="DE19" t="n">
+      <c r="DF19" t="n">
         <v>0.6506180871828237</v>
-      </c>
-      <c r="DF19" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG19" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH19" t="inlineStr"/>
-      <c r="DI19" t="n">
-        <v>0.03384945695610326</v>
-      </c>
-      <c r="DJ19" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK19" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL19" t="n">
-        <v>1.993203138117973</v>
       </c>
     </row>
     <row r="20">
@@ -6792,35 +6654,47 @@
       <c r="CJ20" t="inlineStr"/>
       <c r="CK20" t="inlineStr"/>
       <c r="CL20" t="inlineStr"/>
-      <c r="CM20" t="inlineStr"/>
-      <c r="CN20" t="inlineStr"/>
-      <c r="CO20" t="inlineStr"/>
-      <c r="CP20" t="inlineStr"/>
-      <c r="CQ20" t="inlineStr"/>
-      <c r="CR20" t="inlineStr"/>
-      <c r="CS20" t="inlineStr"/>
+      <c r="CM20" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN20" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO20" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP20" t="n">
+        <v>0.1657126598552314</v>
+      </c>
+      <c r="CQ20" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR20" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS20" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT20" t="inlineStr"/>
       <c r="CU20" t="inlineStr"/>
       <c r="CV20" t="inlineStr"/>
       <c r="CW20" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX20" t="n">
+      <c r="CX20" t="inlineStr"/>
+      <c r="CY20" t="n">
         <v>0.9995393386604625</v>
       </c>
-      <c r="CY20" t="n">
+      <c r="CZ20" t="n">
         <v>0.7150886164052068</v>
       </c>
-      <c r="CZ20" t="n">
+      <c r="DA20" t="n">
         <v>1.030678318936897</v>
       </c>
-      <c r="DA20" t="inlineStr">
+      <c r="DB20" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB20" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC20" t="n">
         <v>1.299826689774697</v>
@@ -6832,25 +6706,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF20" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG20" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH20" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI20" t="n">
-        <v>0.1657126598552314</v>
-      </c>
-      <c r="DJ20" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK20" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL20" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="21">
@@ -7118,65 +6974,59 @@
       <c r="CJ21" t="inlineStr"/>
       <c r="CK21" t="inlineStr"/>
       <c r="CL21" t="inlineStr"/>
-      <c r="CM21" t="inlineStr"/>
-      <c r="CN21" t="inlineStr"/>
-      <c r="CO21" t="inlineStr"/>
-      <c r="CP21" t="inlineStr"/>
-      <c r="CQ21" t="inlineStr"/>
-      <c r="CR21" t="inlineStr"/>
-      <c r="CS21" t="inlineStr"/>
+      <c r="CM21" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN21" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO21" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP21" t="n">
+        <v>0.02713939632415132</v>
+      </c>
+      <c r="CQ21" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR21" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS21" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT21" t="inlineStr"/>
       <c r="CU21" t="inlineStr"/>
       <c r="CV21" t="inlineStr"/>
       <c r="CW21" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX21" t="n">
+      <c r="CX21" t="inlineStr"/>
+      <c r="CY21" t="n">
         <v>1.014635490411201</v>
       </c>
-      <c r="CY21" t="n">
+      <c r="CZ21" t="n">
         <v>0.9202085928078108</v>
       </c>
-      <c r="CZ21" t="n">
+      <c r="DA21" t="n">
         <v>0.9991555502986639</v>
       </c>
-      <c r="DA21" t="inlineStr">
+      <c r="DB21" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB21" t="n">
-        <v>0.6504065040650406</v>
       </c>
       <c r="DC21" t="n">
         <v>0.6504065040650406</v>
       </c>
       <c r="DD21" t="n">
-        <v>0.6499837504062399</v>
+        <v>0.6504065040650406</v>
       </c>
       <c r="DE21" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DF21" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG21" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH21" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI21" t="n">
-        <v>0.02713939632415132</v>
-      </c>
-      <c r="DJ21" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK21" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL21" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="22">
@@ -7436,63 +7286,57 @@
       <c r="CJ22" t="inlineStr"/>
       <c r="CK22" t="inlineStr"/>
       <c r="CL22" t="inlineStr"/>
-      <c r="CM22" t="inlineStr"/>
-      <c r="CN22" t="inlineStr"/>
+      <c r="CM22" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN22" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO22" t="inlineStr"/>
-      <c r="CP22" t="inlineStr"/>
-      <c r="CQ22" t="inlineStr"/>
-      <c r="CR22" t="inlineStr"/>
-      <c r="CS22" t="inlineStr"/>
+      <c r="CP22" t="n">
+        <v>0.1612922712068134</v>
+      </c>
+      <c r="CQ22" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR22" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS22" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT22" t="inlineStr"/>
       <c r="CU22" t="inlineStr"/>
       <c r="CV22" t="inlineStr"/>
       <c r="CW22" t="n">
         <v>0</v>
       </c>
-      <c r="CX22" t="n">
+      <c r="CX22" t="inlineStr"/>
+      <c r="CY22" t="n">
         <v>1.008164314772437</v>
       </c>
-      <c r="CY22" t="n">
+      <c r="CZ22" t="n">
         <v>0.9741185995116167</v>
       </c>
-      <c r="CZ22" t="n">
+      <c r="DA22" t="n">
         <v>1.002457515769358</v>
       </c>
-      <c r="DA22" t="inlineStr">
+      <c r="DB22" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB22" t="n">
-        <v>1.300108342361864</v>
       </c>
       <c r="DC22" t="n">
         <v>1.300108342361864</v>
       </c>
       <c r="DD22" t="n">
-        <v>1.299826689774697</v>
+        <v>1.300108342361864</v>
       </c>
       <c r="DE22" t="n">
         <v>1.299826689774697</v>
       </c>
       <c r="DF22" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG22" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH22" t="inlineStr"/>
-      <c r="DI22" t="n">
-        <v>0.1612922712068134</v>
-      </c>
-      <c r="DJ22" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK22" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL22" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="23">
@@ -7752,35 +7596,45 @@
       <c r="CJ23" t="inlineStr"/>
       <c r="CK23" t="inlineStr"/>
       <c r="CL23" t="inlineStr"/>
-      <c r="CM23" t="inlineStr"/>
-      <c r="CN23" t="inlineStr"/>
+      <c r="CM23" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN23" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO23" t="inlineStr"/>
-      <c r="CP23" t="inlineStr"/>
-      <c r="CQ23" t="inlineStr"/>
-      <c r="CR23" t="inlineStr"/>
-      <c r="CS23" t="inlineStr"/>
+      <c r="CP23" t="n">
+        <v>0.09777790755039455</v>
+      </c>
+      <c r="CQ23" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR23" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS23" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT23" t="inlineStr"/>
       <c r="CU23" t="inlineStr"/>
       <c r="CV23" t="inlineStr"/>
       <c r="CW23" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX23" t="n">
+      <c r="CX23" t="inlineStr"/>
+      <c r="CY23" t="n">
         <v>1.048673337742408</v>
       </c>
-      <c r="CY23" t="n">
+      <c r="CZ23" t="n">
         <v>0.9559770881732745</v>
       </c>
-      <c r="CZ23" t="n">
+      <c r="DA23" t="n">
         <v>1.187378214994207</v>
       </c>
-      <c r="DA23" t="inlineStr">
+      <c r="DB23" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB23" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC23" t="n">
         <v>1.299826689774697</v>
@@ -7792,23 +7646,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF23" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG23" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH23" t="inlineStr"/>
-      <c r="DI23" t="n">
-        <v>0.09777790755039455</v>
-      </c>
-      <c r="DJ23" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK23" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL23" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="24">
@@ -8076,65 +7914,59 @@
       <c r="CJ24" t="inlineStr"/>
       <c r="CK24" t="inlineStr"/>
       <c r="CL24" t="inlineStr"/>
-      <c r="CM24" t="inlineStr"/>
-      <c r="CN24" t="inlineStr"/>
-      <c r="CO24" t="inlineStr"/>
-      <c r="CP24" t="inlineStr"/>
-      <c r="CQ24" t="inlineStr"/>
-      <c r="CR24" t="inlineStr"/>
-      <c r="CS24" t="inlineStr"/>
+      <c r="CM24" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN24" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO24" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP24" t="n">
+        <v>0.1389639468749126</v>
+      </c>
+      <c r="CQ24" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR24" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS24" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT24" t="inlineStr"/>
       <c r="CU24" t="inlineStr"/>
       <c r="CV24" t="inlineStr"/>
       <c r="CW24" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX24" t="n">
+      <c r="CX24" t="inlineStr"/>
+      <c r="CY24" t="n">
         <v>0.9328998469251686</v>
       </c>
-      <c r="CY24" t="n">
+      <c r="CZ24" t="n">
         <v>0.6513335073858831</v>
       </c>
-      <c r="CZ24" t="n">
+      <c r="DA24" t="n">
         <v>1.079745872736531</v>
       </c>
-      <c r="DA24" t="inlineStr">
+      <c r="DB24" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB24" t="n">
+      <c r="DC24" t="n">
         <v>1.300672013873835</v>
       </c>
-      <c r="DC24" t="n">
+      <c r="DD24" t="n">
         <v>1.300390117035111</v>
-      </c>
-      <c r="DD24" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DE24" t="n">
         <v>1.299826689774697</v>
       </c>
       <c r="DF24" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG24" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH24" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI24" t="n">
-        <v>0.1389639468749126</v>
-      </c>
-      <c r="DJ24" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK24" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL24" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="25">
@@ -8394,63 +8226,57 @@
       <c r="CJ25" t="inlineStr"/>
       <c r="CK25" t="inlineStr"/>
       <c r="CL25" t="inlineStr"/>
-      <c r="CM25" t="inlineStr"/>
-      <c r="CN25" t="inlineStr"/>
+      <c r="CM25" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN25" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO25" t="inlineStr"/>
-      <c r="CP25" t="inlineStr"/>
-      <c r="CQ25" t="inlineStr"/>
-      <c r="CR25" t="inlineStr"/>
-      <c r="CS25" t="inlineStr"/>
+      <c r="CP25" t="n">
+        <v>0.1870733326866996</v>
+      </c>
+      <c r="CQ25" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR25" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS25" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT25" t="inlineStr"/>
       <c r="CU25" t="inlineStr"/>
       <c r="CV25" t="inlineStr"/>
       <c r="CW25" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX25" t="n">
+      <c r="CX25" t="inlineStr"/>
+      <c r="CY25" t="n">
         <v>1.004976346083953</v>
       </c>
-      <c r="CY25" t="n">
+      <c r="CZ25" t="n">
         <v>0.98285471377303</v>
       </c>
-      <c r="CZ25" t="n">
+      <c r="DA25" t="n">
         <v>1.04591769446072</v>
       </c>
-      <c r="DA25" t="inlineStr">
+      <c r="DB25" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB25" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC25" t="n">
         <v>1.299826689774697</v>
       </c>
       <c r="DD25" t="n">
-        <v>1.300390117035111</v>
+        <v>1.299826689774697</v>
       </c>
       <c r="DE25" t="n">
         <v>1.300390117035111</v>
       </c>
       <c r="DF25" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG25" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH25" t="inlineStr"/>
-      <c r="DI25" t="n">
-        <v>0.1870733326866996</v>
-      </c>
-      <c r="DJ25" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK25" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL25" t="n">
-        <v>1.19970570478913</v>
+        <v>1.300390117035111</v>
       </c>
     </row>
     <row r="26">
@@ -8718,65 +8544,59 @@
       <c r="CJ26" t="inlineStr"/>
       <c r="CK26" t="inlineStr"/>
       <c r="CL26" t="inlineStr"/>
-      <c r="CM26" t="inlineStr"/>
-      <c r="CN26" t="inlineStr"/>
-      <c r="CO26" t="inlineStr"/>
-      <c r="CP26" t="inlineStr"/>
-      <c r="CQ26" t="inlineStr"/>
-      <c r="CR26" t="inlineStr"/>
-      <c r="CS26" t="inlineStr"/>
+      <c r="CM26" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN26" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO26" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP26" t="n">
+        <v>0.040804065571573</v>
+      </c>
+      <c r="CQ26" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR26" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS26" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT26" t="inlineStr"/>
       <c r="CU26" t="inlineStr"/>
       <c r="CV26" t="inlineStr"/>
       <c r="CW26" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX26" t="n">
+      <c r="CX26" t="inlineStr"/>
+      <c r="CY26" t="n">
         <v>0.9916776239075402</v>
       </c>
-      <c r="CY26" t="n">
+      <c r="CZ26" t="n">
         <v>0.9683088860691933</v>
       </c>
-      <c r="CZ26" t="n">
+      <c r="DA26" t="n">
         <v>1.00335389898459</v>
       </c>
-      <c r="DA26" t="inlineStr">
+      <c r="DB26" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB26" t="n">
+      <c r="DC26" t="n">
         <v>0.6503360069369173</v>
       </c>
-      <c r="DC26" t="n">
+      <c r="DD26" t="n">
         <v>0.6502655250894115</v>
-      </c>
-      <c r="DD26" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DE26" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DF26" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG26" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH26" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI26" t="n">
-        <v>0.040804065571573</v>
-      </c>
-      <c r="DJ26" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK26" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL26" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="27">
@@ -9044,35 +8864,47 @@
       <c r="CJ27" t="inlineStr"/>
       <c r="CK27" t="inlineStr"/>
       <c r="CL27" t="inlineStr"/>
-      <c r="CM27" t="inlineStr"/>
-      <c r="CN27" t="inlineStr"/>
-      <c r="CO27" t="inlineStr"/>
-      <c r="CP27" t="inlineStr"/>
-      <c r="CQ27" t="inlineStr"/>
-      <c r="CR27" t="inlineStr"/>
-      <c r="CS27" t="inlineStr"/>
+      <c r="CM27" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN27" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO27" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP27" t="n">
+        <v>0.06200714219004456</v>
+      </c>
+      <c r="CQ27" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR27" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS27" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT27" t="inlineStr"/>
       <c r="CU27" t="inlineStr"/>
       <c r="CV27" t="inlineStr"/>
       <c r="CW27" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX27" t="n">
+      <c r="CX27" t="inlineStr"/>
+      <c r="CY27" t="n">
         <v>0.9999033140130243</v>
       </c>
-      <c r="CY27" t="n">
+      <c r="CZ27" t="n">
         <v>0.5634703957094437</v>
       </c>
-      <c r="CZ27" t="n">
+      <c r="DA27" t="n">
         <v>1.071986158578824</v>
       </c>
-      <c r="DA27" t="inlineStr">
+      <c r="DB27" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB27" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC27" t="n">
         <v>1.299826689774697</v>
@@ -9084,25 +8916,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF27" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG27" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH27" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI27" t="n">
-        <v>0.06200714219004456</v>
-      </c>
-      <c r="DJ27" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK27" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL27" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="28">
@@ -9362,35 +9176,45 @@
       <c r="CJ28" t="inlineStr"/>
       <c r="CK28" t="inlineStr"/>
       <c r="CL28" t="inlineStr"/>
-      <c r="CM28" t="inlineStr"/>
-      <c r="CN28" t="inlineStr"/>
+      <c r="CM28" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN28" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO28" t="inlineStr"/>
-      <c r="CP28" t="inlineStr"/>
-      <c r="CQ28" t="inlineStr"/>
-      <c r="CR28" t="inlineStr"/>
-      <c r="CS28" t="inlineStr"/>
+      <c r="CP28" t="n">
+        <v>0.05589740593532883</v>
+      </c>
+      <c r="CQ28" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR28" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS28" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT28" t="inlineStr"/>
       <c r="CU28" t="inlineStr"/>
       <c r="CV28" t="inlineStr"/>
       <c r="CW28" t="n">
         <v>0</v>
       </c>
-      <c r="CX28" t="n">
+      <c r="CX28" t="inlineStr"/>
+      <c r="CY28" t="n">
         <v>0.9874345447860932</v>
       </c>
-      <c r="CY28" t="n">
+      <c r="CZ28" t="n">
         <v>0.9831597025203702</v>
       </c>
-      <c r="CZ28" t="n">
+      <c r="DA28" t="n">
         <v>1.008419267322489</v>
       </c>
-      <c r="DA28" t="inlineStr">
+      <c r="DB28" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB28" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC28" t="n">
         <v>1.299826689774697</v>
@@ -9402,23 +9226,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF28" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG28" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH28" t="inlineStr"/>
-      <c r="DI28" t="n">
-        <v>0.05589740593532883</v>
-      </c>
-      <c r="DJ28" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK28" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL28" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="29">
@@ -9686,35 +9494,47 @@
       <c r="CJ29" t="inlineStr"/>
       <c r="CK29" t="inlineStr"/>
       <c r="CL29" t="inlineStr"/>
-      <c r="CM29" t="inlineStr"/>
-      <c r="CN29" t="inlineStr"/>
-      <c r="CO29" t="inlineStr"/>
-      <c r="CP29" t="inlineStr"/>
-      <c r="CQ29" t="inlineStr"/>
-      <c r="CR29" t="inlineStr"/>
-      <c r="CS29" t="inlineStr"/>
+      <c r="CM29" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN29" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO29" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP29" t="n">
+        <v>0.02232383980246641</v>
+      </c>
+      <c r="CQ29" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR29" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS29" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT29" t="inlineStr"/>
       <c r="CU29" t="inlineStr"/>
       <c r="CV29" t="inlineStr"/>
       <c r="CW29" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX29" t="n">
+      <c r="CX29" t="inlineStr"/>
+      <c r="CY29" t="n">
         <v>1.036116646443266</v>
       </c>
-      <c r="CY29" t="n">
+      <c r="CZ29" t="n">
         <v>0.9726428393738623</v>
       </c>
-      <c r="CZ29" t="n">
+      <c r="DA29" t="n">
         <v>0.9973264385216895</v>
       </c>
-      <c r="DA29" t="inlineStr">
+      <c r="DB29" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB29" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC29" t="n">
         <v>0.6499837504062399</v>
@@ -9726,25 +9546,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF29" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG29" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH29" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI29" t="n">
-        <v>0.02232383980246641</v>
-      </c>
-      <c r="DJ29" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK29" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL29" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="30">
@@ -10004,35 +9806,45 @@
       <c r="CJ30" t="inlineStr"/>
       <c r="CK30" t="inlineStr"/>
       <c r="CL30" t="inlineStr"/>
-      <c r="CM30" t="inlineStr"/>
-      <c r="CN30" t="inlineStr"/>
+      <c r="CM30" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN30" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO30" t="inlineStr"/>
-      <c r="CP30" t="inlineStr"/>
-      <c r="CQ30" t="inlineStr"/>
-      <c r="CR30" t="inlineStr"/>
-      <c r="CS30" t="inlineStr"/>
+      <c r="CP30" t="n">
+        <v>0.01973185656702632</v>
+      </c>
+      <c r="CQ30" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR30" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS30" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT30" t="inlineStr"/>
       <c r="CU30" t="inlineStr"/>
       <c r="CV30" t="inlineStr"/>
       <c r="CW30" t="n">
         <v>0</v>
       </c>
-      <c r="CX30" t="n">
+      <c r="CX30" t="inlineStr"/>
+      <c r="CY30" t="n">
         <v>1.035684475293497</v>
       </c>
-      <c r="CY30" t="n">
+      <c r="CZ30" t="n">
         <v>0.973919830742411</v>
       </c>
-      <c r="CZ30" t="n">
+      <c r="DA30" t="n">
         <v>1.002319202088585</v>
       </c>
-      <c r="DA30" t="inlineStr">
+      <c r="DB30" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB30" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC30" t="n">
         <v>0.6499837504062399</v>
@@ -10044,23 +9856,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF30" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG30" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH30" t="inlineStr"/>
-      <c r="DI30" t="n">
-        <v>0.01973185656702632</v>
-      </c>
-      <c r="DJ30" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK30" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL30" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="31">
@@ -10328,35 +10124,47 @@
       <c r="CJ31" t="inlineStr"/>
       <c r="CK31" t="inlineStr"/>
       <c r="CL31" t="inlineStr"/>
-      <c r="CM31" t="inlineStr"/>
-      <c r="CN31" t="inlineStr"/>
-      <c r="CO31" t="inlineStr"/>
-      <c r="CP31" t="inlineStr"/>
-      <c r="CQ31" t="inlineStr"/>
-      <c r="CR31" t="inlineStr"/>
-      <c r="CS31" t="inlineStr"/>
+      <c r="CM31" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN31" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO31" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP31" t="n">
+        <v>0.06178671849733349</v>
+      </c>
+      <c r="CQ31" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR31" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS31" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT31" t="inlineStr"/>
       <c r="CU31" t="inlineStr"/>
       <c r="CV31" t="inlineStr"/>
       <c r="CW31" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX31" t="n">
+      <c r="CX31" t="inlineStr"/>
+      <c r="CY31" t="n">
         <v>0.9993886379694573</v>
       </c>
-      <c r="CY31" t="n">
+      <c r="CZ31" t="n">
         <v>0.6019282542200509</v>
       </c>
-      <c r="CZ31" t="n">
+      <c r="DA31" t="n">
         <v>1.031366932185891</v>
       </c>
-      <c r="DA31" t="inlineStr">
+      <c r="DB31" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB31" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC31" t="n">
         <v>1.299826689774697</v>
@@ -10368,25 +10176,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF31" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG31" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH31" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI31" t="n">
-        <v>0.06178671849733349</v>
-      </c>
-      <c r="DJ31" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK31" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL31" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="32">
@@ -10654,65 +10444,59 @@
       <c r="CJ32" t="inlineStr"/>
       <c r="CK32" t="inlineStr"/>
       <c r="CL32" t="inlineStr"/>
-      <c r="CM32" t="inlineStr"/>
-      <c r="CN32" t="inlineStr"/>
-      <c r="CO32" t="inlineStr"/>
-      <c r="CP32" t="inlineStr"/>
-      <c r="CQ32" t="inlineStr"/>
-      <c r="CR32" t="inlineStr"/>
-      <c r="CS32" t="inlineStr"/>
+      <c r="CM32" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN32" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO32" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP32" t="n">
+        <v>0.04096562911158437</v>
+      </c>
+      <c r="CQ32" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR32" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS32" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT32" t="inlineStr"/>
       <c r="CU32" t="inlineStr"/>
       <c r="CV32" t="inlineStr"/>
       <c r="CW32" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX32" t="n">
+      <c r="CX32" t="inlineStr"/>
+      <c r="CY32" t="n">
         <v>1.001947011801571</v>
       </c>
-      <c r="CY32" t="n">
+      <c r="CZ32" t="n">
         <v>0.9694990787805623</v>
       </c>
-      <c r="CZ32" t="n">
+      <c r="DA32" t="n">
         <v>1.004404093620587</v>
       </c>
-      <c r="DA32" t="inlineStr">
+      <c r="DB32" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB32" t="n">
-        <v>0.6501246072163831</v>
       </c>
       <c r="DC32" t="n">
         <v>0.6501246072163831</v>
       </c>
       <c r="DD32" t="n">
-        <v>0.6499837504062399</v>
+        <v>0.6501246072163831</v>
       </c>
       <c r="DE32" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DF32" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG32" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH32" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI32" t="n">
-        <v>0.04096562911158437</v>
-      </c>
-      <c r="DJ32" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK32" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL32" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="33">
@@ -10972,63 +10756,57 @@
       <c r="CJ33" t="inlineStr"/>
       <c r="CK33" t="inlineStr"/>
       <c r="CL33" t="inlineStr"/>
-      <c r="CM33" t="inlineStr"/>
-      <c r="CN33" t="inlineStr"/>
+      <c r="CM33" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN33" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO33" t="inlineStr"/>
-      <c r="CP33" t="inlineStr"/>
-      <c r="CQ33" t="inlineStr"/>
-      <c r="CR33" t="inlineStr"/>
-      <c r="CS33" t="inlineStr"/>
+      <c r="CP33" t="n">
+        <v>0.03928688455443337</v>
+      </c>
+      <c r="CQ33" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR33" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS33" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT33" t="inlineStr"/>
       <c r="CU33" t="inlineStr"/>
       <c r="CV33" t="inlineStr"/>
       <c r="CW33" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX33" t="n">
+      <c r="CX33" t="inlineStr"/>
+      <c r="CY33" t="n">
         <v>0.9900838225975505</v>
       </c>
-      <c r="CY33" t="n">
+      <c r="CZ33" t="n">
         <v>1.004517644894049</v>
       </c>
-      <c r="CZ33" t="n">
+      <c r="DA33" t="n">
         <v>1.013272637706423</v>
       </c>
-      <c r="DA33" t="inlineStr">
+      <c r="DB33" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB33" t="n">
-        <v>0.6501246072163831</v>
       </c>
       <c r="DC33" t="n">
         <v>0.6501246072163831</v>
       </c>
       <c r="DD33" t="n">
+        <v>0.6501246072163831</v>
+      </c>
+      <c r="DE33" t="n">
         <v>0.6506886454831363</v>
       </c>
-      <c r="DE33" t="n">
+      <c r="DF33" t="n">
         <v>0.6502655250894115</v>
-      </c>
-      <c r="DF33" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG33" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH33" t="inlineStr"/>
-      <c r="DI33" t="n">
-        <v>0.03928688455443337</v>
-      </c>
-      <c r="DJ33" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK33" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL33" t="n">
-        <v>1.993203138117973</v>
       </c>
     </row>
     <row r="34">
@@ -11288,35 +11066,45 @@
       <c r="CJ34" t="inlineStr"/>
       <c r="CK34" t="inlineStr"/>
       <c r="CL34" t="inlineStr"/>
-      <c r="CM34" t="inlineStr"/>
-      <c r="CN34" t="inlineStr"/>
+      <c r="CM34" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN34" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO34" t="inlineStr"/>
-      <c r="CP34" t="inlineStr"/>
-      <c r="CQ34" t="inlineStr"/>
-      <c r="CR34" t="inlineStr"/>
-      <c r="CS34" t="inlineStr"/>
+      <c r="CP34" t="n">
+        <v>0.01013229810217492</v>
+      </c>
+      <c r="CQ34" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR34" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS34" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT34" t="inlineStr"/>
       <c r="CU34" t="inlineStr"/>
       <c r="CV34" t="inlineStr"/>
       <c r="CW34" t="n">
         <v>0</v>
       </c>
-      <c r="CX34" t="n">
+      <c r="CX34" t="inlineStr"/>
+      <c r="CY34" t="n">
         <v>1.050675557659946</v>
       </c>
-      <c r="CY34" t="n">
+      <c r="CZ34" t="n">
         <v>0.9727398932970273</v>
       </c>
-      <c r="CZ34" t="n">
+      <c r="DA34" t="n">
         <v>1.005223990273701</v>
       </c>
-      <c r="DA34" t="inlineStr">
+      <c r="DB34" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB34" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC34" t="n">
         <v>0.6499837504062399</v>
@@ -11328,23 +11116,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF34" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG34" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH34" t="inlineStr"/>
-      <c r="DI34" t="n">
-        <v>0.01013229810217492</v>
-      </c>
-      <c r="DJ34" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK34" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL34" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="35">
@@ -11612,35 +11384,47 @@
       <c r="CJ35" t="inlineStr"/>
       <c r="CK35" t="inlineStr"/>
       <c r="CL35" t="inlineStr"/>
-      <c r="CM35" t="inlineStr"/>
-      <c r="CN35" t="inlineStr"/>
-      <c r="CO35" t="inlineStr"/>
-      <c r="CP35" t="inlineStr"/>
-      <c r="CQ35" t="inlineStr"/>
-      <c r="CR35" t="inlineStr"/>
-      <c r="CS35" t="inlineStr"/>
+      <c r="CM35" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN35" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO35" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP35" t="n">
+        <v>0.1133037354504893</v>
+      </c>
+      <c r="CQ35" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR35" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS35" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT35" t="inlineStr"/>
       <c r="CU35" t="inlineStr"/>
       <c r="CV35" t="inlineStr"/>
       <c r="CW35" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX35" t="n">
+      <c r="CX35" t="inlineStr"/>
+      <c r="CY35" t="n">
         <v>0.9546863800892419</v>
       </c>
-      <c r="CY35" t="n">
+      <c r="CZ35" t="n">
         <v>0.6959003484633897</v>
       </c>
-      <c r="CZ35" t="n">
+      <c r="DA35" t="n">
         <v>1.005276593475788</v>
       </c>
-      <c r="DA35" t="inlineStr">
+      <c r="DB35" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB35" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC35" t="n">
         <v>1.299826689774697</v>
@@ -11652,25 +11436,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF35" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG35" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH35" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI35" t="n">
-        <v>0.1133037354504893</v>
-      </c>
-      <c r="DJ35" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK35" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL35" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="36">
@@ -11930,35 +11696,45 @@
       <c r="CJ36" t="inlineStr"/>
       <c r="CK36" t="inlineStr"/>
       <c r="CL36" t="inlineStr"/>
-      <c r="CM36" t="inlineStr"/>
-      <c r="CN36" t="inlineStr"/>
+      <c r="CM36" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN36" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO36" t="inlineStr"/>
-      <c r="CP36" t="inlineStr"/>
-      <c r="CQ36" t="inlineStr"/>
-      <c r="CR36" t="inlineStr"/>
-      <c r="CS36" t="inlineStr"/>
+      <c r="CP36" t="n">
+        <v>0.1088331344550831</v>
+      </c>
+      <c r="CQ36" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR36" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS36" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT36" t="inlineStr"/>
       <c r="CU36" t="inlineStr"/>
       <c r="CV36" t="inlineStr"/>
       <c r="CW36" t="n">
         <v>0</v>
       </c>
-      <c r="CX36" t="n">
+      <c r="CX36" t="inlineStr"/>
+      <c r="CY36" t="n">
         <v>0.9873321705367474</v>
       </c>
-      <c r="CY36" t="n">
+      <c r="CZ36" t="n">
         <v>0.9879995515699611</v>
       </c>
-      <c r="CZ36" t="n">
+      <c r="DA36" t="n">
         <v>1.000711966559532</v>
       </c>
-      <c r="DA36" t="inlineStr">
+      <c r="DB36" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB36" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC36" t="n">
         <v>1.299826689774697</v>
@@ -11970,23 +11746,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF36" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG36" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH36" t="inlineStr"/>
-      <c r="DI36" t="n">
-        <v>0.1088331344550831</v>
-      </c>
-      <c r="DJ36" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK36" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL36" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="37">
@@ -12254,38 +12014,50 @@
       <c r="CJ37" t="inlineStr"/>
       <c r="CK37" t="inlineStr"/>
       <c r="CL37" t="inlineStr"/>
-      <c r="CM37" t="inlineStr"/>
-      <c r="CN37" t="inlineStr"/>
-      <c r="CO37" t="inlineStr"/>
-      <c r="CP37" t="inlineStr"/>
-      <c r="CQ37" t="inlineStr"/>
-      <c r="CR37" t="inlineStr"/>
-      <c r="CS37" t="inlineStr"/>
+      <c r="CM37" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN37" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO37" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP37" t="n">
+        <v>0.01252808972117762</v>
+      </c>
+      <c r="CQ37" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR37" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS37" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT37" t="inlineStr"/>
       <c r="CU37" t="inlineStr"/>
       <c r="CV37" t="inlineStr"/>
       <c r="CW37" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX37" t="n">
+      <c r="CX37" t="inlineStr"/>
+      <c r="CY37" t="n">
         <v>1.076967236710759</v>
       </c>
-      <c r="CY37" t="n">
+      <c r="CZ37" t="n">
         <v>0.9350076791826907</v>
       </c>
-      <c r="CZ37" t="n">
+      <c r="DA37" t="n">
         <v>1.003671852066075</v>
       </c>
-      <c r="DA37" t="inlineStr">
+      <c r="DB37" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB37" t="n">
+      <c r="DC37" t="n">
         <v>0.6500541711809318</v>
-      </c>
-      <c r="DC37" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DD37" t="n">
         <v>0.6499837504062399</v>
@@ -12294,25 +12066,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF37" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG37" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH37" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI37" t="n">
-        <v>0.01252808972117762</v>
-      </c>
-      <c r="DJ37" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK37" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL37" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="38">
@@ -12580,35 +12334,47 @@
       <c r="CJ38" t="inlineStr"/>
       <c r="CK38" t="inlineStr"/>
       <c r="CL38" t="inlineStr"/>
-      <c r="CM38" t="inlineStr"/>
-      <c r="CN38" t="inlineStr"/>
-      <c r="CO38" t="inlineStr"/>
-      <c r="CP38" t="inlineStr"/>
-      <c r="CQ38" t="inlineStr"/>
-      <c r="CR38" t="inlineStr"/>
-      <c r="CS38" t="inlineStr"/>
+      <c r="CM38" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN38" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO38" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP38" t="n">
+        <v>0.1947558217758928</v>
+      </c>
+      <c r="CQ38" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR38" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS38" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT38" t="inlineStr"/>
       <c r="CU38" t="inlineStr"/>
       <c r="CV38" t="inlineStr"/>
       <c r="CW38" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX38" t="n">
+      <c r="CX38" t="inlineStr"/>
+      <c r="CY38" t="n">
         <v>0.9439121155247246</v>
       </c>
-      <c r="CY38" t="n">
+      <c r="CZ38" t="n">
         <v>0.6850309107829227</v>
       </c>
-      <c r="CZ38" t="n">
+      <c r="DA38" t="n">
         <v>1.032962861134033</v>
       </c>
-      <c r="DA38" t="inlineStr">
+      <c r="DB38" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB38" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC38" t="n">
         <v>1.299826689774697</v>
@@ -12620,25 +12386,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF38" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG38" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH38" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI38" t="n">
-        <v>0.1947558217758928</v>
-      </c>
-      <c r="DJ38" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK38" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL38" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="39">
@@ -12898,35 +12646,45 @@
       <c r="CJ39" t="inlineStr"/>
       <c r="CK39" t="inlineStr"/>
       <c r="CL39" t="inlineStr"/>
-      <c r="CM39" t="inlineStr"/>
-      <c r="CN39" t="inlineStr"/>
+      <c r="CM39" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN39" t="n">
+        <v>0.922850542145485</v>
+      </c>
       <c r="CO39" t="inlineStr"/>
-      <c r="CP39" t="inlineStr"/>
-      <c r="CQ39" t="inlineStr"/>
-      <c r="CR39" t="inlineStr"/>
-      <c r="CS39" t="inlineStr"/>
+      <c r="CP39" t="n">
+        <v>0.1381971447624315</v>
+      </c>
+      <c r="CQ39" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR39" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS39" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT39" t="inlineStr"/>
       <c r="CU39" t="inlineStr"/>
       <c r="CV39" t="inlineStr"/>
       <c r="CW39" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX39" t="n">
+      <c r="CX39" t="inlineStr"/>
+      <c r="CY39" t="n">
         <v>1.007144305009835</v>
       </c>
-      <c r="CY39" t="n">
+      <c r="CZ39" t="n">
         <v>1.001446744042854</v>
       </c>
-      <c r="CZ39" t="n">
+      <c r="DA39" t="n">
         <v>1.02662651612981</v>
       </c>
-      <c r="DA39" t="inlineStr">
+      <c r="DB39" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB39" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC39" t="n">
         <v>1.299826689774697</v>
@@ -12938,23 +12696,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF39" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG39" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH39" t="inlineStr"/>
-      <c r="DI39" t="n">
-        <v>0.1381971447624315</v>
-      </c>
-      <c r="DJ39" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK39" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL39" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="40">
@@ -13222,35 +12964,47 @@
       <c r="CJ40" t="inlineStr"/>
       <c r="CK40" t="inlineStr"/>
       <c r="CL40" t="inlineStr"/>
-      <c r="CM40" t="inlineStr"/>
-      <c r="CN40" t="inlineStr"/>
-      <c r="CO40" t="inlineStr"/>
-      <c r="CP40" t="inlineStr"/>
-      <c r="CQ40" t="inlineStr"/>
-      <c r="CR40" t="inlineStr"/>
-      <c r="CS40" t="inlineStr"/>
+      <c r="CM40" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN40" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO40" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP40" t="n">
+        <v>0.03128820869973956</v>
+      </c>
+      <c r="CQ40" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR40" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS40" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT40" t="inlineStr"/>
       <c r="CU40" t="inlineStr"/>
       <c r="CV40" t="inlineStr"/>
       <c r="CW40" t="n">
         <v>3.8</v>
       </c>
-      <c r="CX40" t="n">
+      <c r="CX40" t="inlineStr"/>
+      <c r="CY40" t="n">
         <v>1.038855785172671</v>
       </c>
-      <c r="CY40" t="n">
+      <c r="CZ40" t="n">
         <v>0.9692653470850712</v>
       </c>
-      <c r="CZ40" t="n">
+      <c r="DA40" t="n">
         <v>0.9994864585626243</v>
       </c>
-      <c r="DA40" t="inlineStr">
+      <c r="DB40" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB40" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC40" t="n">
         <v>0.6499837504062399</v>
@@ -13262,25 +13016,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF40" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG40" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH40" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI40" t="n">
-        <v>0.03128820869973956</v>
-      </c>
-      <c r="DJ40" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK40" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL40" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="41">
@@ -13548,35 +13284,47 @@
       <c r="CJ41" t="inlineStr"/>
       <c r="CK41" t="inlineStr"/>
       <c r="CL41" t="inlineStr"/>
-      <c r="CM41" t="inlineStr"/>
-      <c r="CN41" t="inlineStr"/>
-      <c r="CO41" t="inlineStr"/>
-      <c r="CP41" t="inlineStr"/>
-      <c r="CQ41" t="inlineStr"/>
-      <c r="CR41" t="inlineStr"/>
-      <c r="CS41" t="inlineStr"/>
+      <c r="CM41" t="n">
+        <v>6.80845382890728</v>
+      </c>
+      <c r="CN41" t="n">
+        <v>0.922850542145485</v>
+      </c>
+      <c r="CO41" t="n">
+        <v>17.83814903173707</v>
+      </c>
+      <c r="CP41" t="n">
+        <v>0.1004127791821821</v>
+      </c>
+      <c r="CQ41" t="n">
+        <v>3.948903220766222</v>
+      </c>
+      <c r="CR41" t="n">
+        <v>0.9992571606462729</v>
+      </c>
+      <c r="CS41" t="n">
+        <v>1.19970570478913</v>
+      </c>
       <c r="CT41" t="inlineStr"/>
       <c r="CU41" t="inlineStr"/>
       <c r="CV41" t="inlineStr"/>
       <c r="CW41" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX41" t="n">
+      <c r="CX41" t="inlineStr"/>
+      <c r="CY41" t="n">
         <v>1.112204962588671</v>
       </c>
-      <c r="CY41" t="n">
+      <c r="CZ41" t="n">
         <v>0.7024103951713738</v>
       </c>
-      <c r="CZ41" t="n">
+      <c r="DA41" t="n">
         <v>1.002684043088939</v>
       </c>
-      <c r="DA41" t="inlineStr">
+      <c r="DB41" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB41" t="n">
-        <v>1.299826689774697</v>
       </c>
       <c r="DC41" t="n">
         <v>1.299826689774697</v>
@@ -13588,25 +13336,7 @@
         <v>1.299826689774697</v>
       </c>
       <c r="DF41" t="n">
-        <v>6.80845382890728</v>
-      </c>
-      <c r="DG41" t="n">
-        <v>0.922850542145485</v>
-      </c>
-      <c r="DH41" t="n">
-        <v>17.83814903173707</v>
-      </c>
-      <c r="DI41" t="n">
-        <v>0.1004127791821821</v>
-      </c>
-      <c r="DJ41" t="n">
-        <v>3.948903220766222</v>
-      </c>
-      <c r="DK41" t="n">
-        <v>0.9992571606462729</v>
-      </c>
-      <c r="DL41" t="n">
-        <v>1.19970570478913</v>
+        <v>1.299826689774697</v>
       </c>
     </row>
     <row r="42">
@@ -13866,35 +13596,45 @@
       <c r="CJ42" t="inlineStr"/>
       <c r="CK42" t="inlineStr"/>
       <c r="CL42" t="inlineStr"/>
-      <c r="CM42" t="inlineStr"/>
-      <c r="CN42" t="inlineStr"/>
+      <c r="CM42" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN42" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO42" t="inlineStr"/>
-      <c r="CP42" t="inlineStr"/>
-      <c r="CQ42" t="inlineStr"/>
-      <c r="CR42" t="inlineStr"/>
-      <c r="CS42" t="inlineStr"/>
+      <c r="CP42" t="n">
+        <v>0.02906504521321584</v>
+      </c>
+      <c r="CQ42" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR42" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS42" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT42" t="inlineStr"/>
       <c r="CU42" t="inlineStr"/>
       <c r="CV42" t="inlineStr"/>
       <c r="CW42" t="n">
         <v>0</v>
       </c>
-      <c r="CX42" t="n">
+      <c r="CX42" t="inlineStr"/>
+      <c r="CY42" t="n">
         <v>1.032928706432218</v>
       </c>
-      <c r="CY42" t="n">
+      <c r="CZ42" t="n">
         <v>0.9821967826360616</v>
       </c>
-      <c r="CZ42" t="n">
+      <c r="DA42" t="n">
         <v>0.9992322314944626</v>
       </c>
-      <c r="DA42" t="inlineStr">
+      <c r="DB42" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB42" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DC42" t="n">
         <v>0.6499837504062399</v>
@@ -13906,23 +13646,7 @@
         <v>0.6499837504062399</v>
       </c>
       <c r="DF42" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG42" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH42" t="inlineStr"/>
-      <c r="DI42" t="n">
-        <v>0.02906504521321584</v>
-      </c>
-      <c r="DJ42" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK42" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL42" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
     <row r="43">
@@ -14182,63 +13906,57 @@
       <c r="CJ43" t="inlineStr"/>
       <c r="CK43" t="inlineStr"/>
       <c r="CL43" t="inlineStr"/>
-      <c r="CM43" t="inlineStr"/>
-      <c r="CN43" t="inlineStr"/>
+      <c r="CM43" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN43" t="n">
+        <v>3.066466366335344</v>
+      </c>
       <c r="CO43" t="inlineStr"/>
-      <c r="CP43" t="inlineStr"/>
-      <c r="CQ43" t="inlineStr"/>
-      <c r="CR43" t="inlineStr"/>
-      <c r="CS43" t="inlineStr"/>
+      <c r="CP43" t="n">
+        <v>0.02802005592461942</v>
+      </c>
+      <c r="CQ43" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR43" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS43" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT43" t="inlineStr"/>
       <c r="CU43" t="inlineStr"/>
       <c r="CV43" t="inlineStr"/>
       <c r="CW43" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX43" t="n">
+      <c r="CX43" t="inlineStr"/>
+      <c r="CY43" t="n">
         <v>1.064495383364179</v>
       </c>
-      <c r="CY43" t="n">
+      <c r="CZ43" t="n">
         <v>0.9811418953926931</v>
       </c>
-      <c r="CZ43" t="n">
+      <c r="DA43" t="n">
         <v>0.8904893205450086</v>
       </c>
-      <c r="DA43" t="inlineStr">
+      <c r="DB43" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
-      </c>
-      <c r="DB43" t="n">
-        <v>0.6501246072163831</v>
       </c>
       <c r="DC43" t="n">
         <v>0.6501246072163831</v>
       </c>
       <c r="DD43" t="n">
-        <v>0.6502655250894115</v>
+        <v>0.6501246072163831</v>
       </c>
       <c r="DE43" t="n">
         <v>0.6502655250894115</v>
       </c>
       <c r="DF43" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG43" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH43" t="inlineStr"/>
-      <c r="DI43" t="n">
-        <v>0.02802005592461942</v>
-      </c>
-      <c r="DJ43" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK43" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL43" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6502655250894115</v>
       </c>
     </row>
     <row r="44">
@@ -14506,65 +14224,59 @@
       <c r="CJ44" t="inlineStr"/>
       <c r="CK44" t="inlineStr"/>
       <c r="CL44" t="inlineStr"/>
-      <c r="CM44" t="inlineStr"/>
-      <c r="CN44" t="inlineStr"/>
-      <c r="CO44" t="inlineStr"/>
-      <c r="CP44" t="inlineStr"/>
-      <c r="CQ44" t="inlineStr"/>
-      <c r="CR44" t="inlineStr"/>
-      <c r="CS44" t="inlineStr"/>
+      <c r="CM44" t="n">
+        <v>2.048998605091</v>
+      </c>
+      <c r="CN44" t="n">
+        <v>3.066466366335344</v>
+      </c>
+      <c r="CO44" t="n">
+        <v>5.368376345338421</v>
+      </c>
+      <c r="CP44" t="n">
+        <v>0.03374577762668574</v>
+      </c>
+      <c r="CQ44" t="n">
+        <v>1.18841919095278</v>
+      </c>
+      <c r="CR44" t="n">
+        <v>0.8300879542525339</v>
+      </c>
+      <c r="CS44" t="n">
+        <v>1.993203138117973</v>
+      </c>
       <c r="CT44" t="inlineStr"/>
       <c r="CU44" t="inlineStr"/>
       <c r="CV44" t="inlineStr"/>
       <c r="CW44" t="n">
         <v>5.8</v>
       </c>
-      <c r="CX44" t="n">
+      <c r="CX44" t="inlineStr"/>
+      <c r="CY44" t="n">
         <v>1.009326342249142</v>
       </c>
-      <c r="CY44" t="n">
+      <c r="CZ44" t="n">
         <v>0.9663191783345513</v>
       </c>
-      <c r="CZ44" t="n">
+      <c r="DA44" t="n">
         <v>1.000837374856073</v>
       </c>
-      <c r="DA44" t="inlineStr">
+      <c r="DB44" t="inlineStr">
         <is>
           <t>PROCESSED-20251112-tett6roof</t>
         </is>
       </c>
-      <c r="DB44" t="n">
+      <c r="DC44" t="n">
         <v>0.6501950585175553</v>
       </c>
-      <c r="DC44" t="n">
+      <c r="DD44" t="n">
         <v>0.6501246072163831</v>
-      </c>
-      <c r="DD44" t="n">
-        <v>0.6499837504062399</v>
       </c>
       <c r="DE44" t="n">
         <v>0.6499837504062399</v>
       </c>
       <c r="DF44" t="n">
-        <v>2.048998605091</v>
-      </c>
-      <c r="DG44" t="n">
-        <v>3.066466366335344</v>
-      </c>
-      <c r="DH44" t="n">
-        <v>5.368376345338421</v>
-      </c>
-      <c r="DI44" t="n">
-        <v>0.03374577762668574</v>
-      </c>
-      <c r="DJ44" t="n">
-        <v>1.18841919095278</v>
-      </c>
-      <c r="DK44" t="n">
-        <v>0.8300879542525339</v>
-      </c>
-      <c r="DL44" t="n">
-        <v>1.993203138117973</v>
+        <v>0.6499837504062399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funker nå, med get_positive_spectrum()
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251112-tett6roof/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251112-tett6roof/meta.xlsx
@@ -1580,7 +1580,7 @@
         <v>1.044162970336802</v>
       </c>
       <c r="CZ3" t="n">
-        <v>0.9696157709281857</v>
+        <v>0.969615770928186</v>
       </c>
       <c r="DA3" t="n">
         <v>1.003088565524012</v>
@@ -1957,7 +1957,7 @@
         <v>9.719999999999999</v>
       </c>
       <c r="BE5" t="n">
-        <v>7.462442189713257</v>
+        <v>7.462442189713259</v>
       </c>
       <c r="BF5" t="n">
         <v>7.394356342484373</v>
@@ -2077,7 +2077,7 @@
         <v>1.014358044141053</v>
       </c>
       <c r="DA5" t="n">
-        <v>1.036939680368307</v>
+        <v>1.036939680368306</v>
       </c>
       <c r="DB5" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>10.83500000000001</v>
       </c>
       <c r="AL7" t="n">
-        <v>9.14801157801171</v>
+        <v>9.148011578011708</v>
       </c>
       <c r="AM7" t="n">
         <v>9.179460294854394</v>
@@ -2701,10 +2701,10 @@
       </c>
       <c r="CX7" t="inlineStr"/>
       <c r="CY7" t="n">
-        <v>1.03709056210268</v>
+        <v>1.037090562102679</v>
       </c>
       <c r="CZ7" t="n">
-        <v>0.9673806146154074</v>
+        <v>0.9673806146154076</v>
       </c>
       <c r="DA7" t="n">
         <v>1.018331230674218</v>
@@ -3115,7 +3115,7 @@
         <v>5.805000000000007</v>
       </c>
       <c r="S9" t="n">
-        <v>4.447034070100692</v>
+        <v>4.44703407010069</v>
       </c>
       <c r="T9" t="n">
         <v>4.467840408626308</v>
@@ -3217,7 +3217,7 @@
         <v>8.639999999999986</v>
       </c>
       <c r="BE9" t="n">
-        <v>4.545460881105915</v>
+        <v>4.545460881105916</v>
       </c>
       <c r="BF9" t="n">
         <v>4.595381212169954</v>
@@ -3334,10 +3334,10 @@
         <v>1.019573777652404</v>
       </c>
       <c r="CZ9" t="n">
-        <v>1.002510224035701</v>
+        <v>1.002510224035702</v>
       </c>
       <c r="DA9" t="n">
-        <v>0.9787999311488548</v>
+        <v>0.9787999311488547</v>
       </c>
       <c r="DB9" t="inlineStr">
         <is>
@@ -4065,7 +4065,7 @@
         <v>5.805000000000007</v>
       </c>
       <c r="S12" t="n">
-        <v>4.422158802810139</v>
+        <v>4.42215880281014</v>
       </c>
       <c r="T12" t="n">
         <v>4.483331558359191</v>
@@ -4218,7 +4218,7 @@
         <v>8.640000000000015</v>
       </c>
       <c r="BX12" t="n">
-        <v>4.553267299642018</v>
+        <v>4.553267299642019</v>
       </c>
       <c r="BY12" t="n">
         <v>4.620145247832278</v>
@@ -4287,7 +4287,7 @@
         <v>1.004577508931341</v>
       </c>
       <c r="DA12" t="n">
-        <v>0.9921151426193191</v>
+        <v>0.9921151426193193</v>
       </c>
       <c r="DB12" t="inlineStr">
         <is>
@@ -4738,7 +4738,7 @@
         <v>9.669999999999987</v>
       </c>
       <c r="AL14" t="n">
-        <v>9.303608996729254</v>
+        <v>9.303608996729253</v>
       </c>
       <c r="AM14" t="n">
         <v>9.327362573040219</v>
@@ -4791,7 +4791,7 @@
         <v>9.455000000000013</v>
       </c>
       <c r="BE14" t="n">
-        <v>9.023349833359681</v>
+        <v>9.02334983335968</v>
       </c>
       <c r="BF14" t="n">
         <v>9.039026508540113</v>
@@ -4844,7 +4844,7 @@
         <v>9.460000000000008</v>
       </c>
       <c r="BX14" t="n">
-        <v>9.030586291021921</v>
+        <v>9.030586291021919</v>
       </c>
       <c r="BY14" t="n">
         <v>9.044213595703551</v>
@@ -4911,7 +4911,7 @@
       </c>
       <c r="CX14" t="inlineStr"/>
       <c r="CY14" t="n">
-        <v>1.049993344681407</v>
+        <v>1.049993344681406</v>
       </c>
       <c r="CZ14" t="n">
         <v>0.9698762960193082</v>
@@ -5736,7 +5736,7 @@
         <v>1.018839537633315</v>
       </c>
       <c r="CZ17" t="n">
-        <v>0.9830592940078693</v>
+        <v>0.9830592940078697</v>
       </c>
       <c r="DA17" t="n">
         <v>1.005635066148295</v>
@@ -6198,7 +6198,7 @@
         <v>16.51999999999997</v>
       </c>
       <c r="AL19" t="n">
-        <v>8.923954467812148</v>
+        <v>8.92395446781215</v>
       </c>
       <c r="AM19" t="n">
         <v>8.954510461360522</v>
@@ -6363,10 +6363,10 @@
       </c>
       <c r="CX19" t="inlineStr"/>
       <c r="CY19" t="n">
-        <v>1.017665842415511</v>
+        <v>1.017665842415512</v>
       </c>
       <c r="CZ19" t="n">
-        <v>0.9589852054503312</v>
+        <v>0.9589852054503311</v>
       </c>
       <c r="DA19" t="n">
         <v>1.035713722053874</v>
@@ -6883,7 +6883,7 @@
         <v>5.074999999999989</v>
       </c>
       <c r="BE21" t="n">
-        <v>4.254206325236899</v>
+        <v>4.254206325236898</v>
       </c>
       <c r="BF21" t="n">
         <v>4.255337511664758</v>
@@ -6936,7 +6936,7 @@
         <v>5.159999999999997</v>
       </c>
       <c r="BX21" t="n">
-        <v>4.25061386197613</v>
+        <v>4.250613861976128</v>
       </c>
       <c r="BY21" t="n">
         <v>4.264233672603522</v>
@@ -7006,10 +7006,10 @@
         <v>1.014635490411201</v>
       </c>
       <c r="CZ21" t="n">
-        <v>0.9202085928078108</v>
+        <v>0.9202085928078105</v>
       </c>
       <c r="DA21" t="n">
-        <v>0.9991555502986639</v>
+        <v>0.9991555502986637</v>
       </c>
       <c r="DB21" t="inlineStr">
         <is>
@@ -8579,7 +8579,7 @@
         <v>0.9683088860691933</v>
       </c>
       <c r="DA26" t="n">
-        <v>1.00335389898459</v>
+        <v>1.003353898984589</v>
       </c>
       <c r="DB26" t="inlineStr">
         <is>
@@ -9297,7 +9297,7 @@
         <v>10.11000000000001</v>
       </c>
       <c r="S29" t="n">
-        <v>8.792347874454222</v>
+        <v>8.792347874454221</v>
       </c>
       <c r="T29" t="n">
         <v>8.792841109601502</v>
@@ -9668,7 +9668,7 @@
         <v>9.629999999999995</v>
       </c>
       <c r="AL30" t="n">
-        <v>9.226775280960016</v>
+        <v>9.226775280960014</v>
       </c>
       <c r="AM30" t="n">
         <v>9.248298619679321</v>
@@ -9719,7 +9719,7 @@
         <v>9.45999999999998</v>
       </c>
       <c r="BE30" t="n">
-        <v>8.98613941993084</v>
+        <v>8.986139419930838</v>
       </c>
       <c r="BF30" t="n">
         <v>8.998321405849786</v>
@@ -10928,7 +10928,7 @@
         <v>4.944999999999965</v>
       </c>
       <c r="AL34" t="n">
-        <v>4.680198781131049</v>
+        <v>4.680198781131048</v>
       </c>
       <c r="AM34" t="n">
         <v>4.690887401888886</v>
@@ -10979,7 +10979,7 @@
         <v>4.734999999999985</v>
       </c>
       <c r="BE34" t="n">
-        <v>4.552616062966293</v>
+        <v>4.552616062966294</v>
       </c>
       <c r="BF34" t="n">
         <v>4.560105683179122</v>
@@ -11030,7 +11030,7 @@
         <v>4.900000000000006</v>
       </c>
       <c r="BX34" t="n">
-        <v>4.576398884999122</v>
+        <v>4.576398884999121</v>
       </c>
       <c r="BY34" t="n">
         <v>4.585062373667363</v>
@@ -11096,10 +11096,10 @@
         <v>1.050675557659946</v>
       </c>
       <c r="CZ34" t="n">
-        <v>0.9727398932970273</v>
+        <v>0.9727398932970276</v>
       </c>
       <c r="DA34" t="n">
-        <v>1.005223990273701</v>
+        <v>1.0052239902737</v>
       </c>
       <c r="DB34" t="inlineStr">
         <is>
@@ -11870,7 +11870,7 @@
         <v>6.114249999999988</v>
       </c>
       <c r="AL37" t="n">
-        <v>4.694313674073984</v>
+        <v>4.694313674073983</v>
       </c>
       <c r="AM37" t="n">
         <v>4.737793021313028</v>
@@ -12046,7 +12046,7 @@
         <v>1.076967236710759</v>
       </c>
       <c r="CZ37" t="n">
-        <v>0.9350076791826907</v>
+        <v>0.935007679182691</v>
       </c>
       <c r="DA37" t="n">
         <v>1.003671852066075</v>
@@ -12767,7 +12767,7 @@
         <v>14.82975000000002</v>
       </c>
       <c r="S40" t="n">
-        <v>13.19721520349957</v>
+        <v>13.19721520349956</v>
       </c>
       <c r="T40" t="n">
         <v>13.21677400229876</v>
@@ -13560,7 +13560,7 @@
         <v>14.56999999999999</v>
       </c>
       <c r="BX42" t="n">
-        <v>13.58162985680418</v>
+        <v>13.58162985680417</v>
       </c>
       <c r="BY42" t="n">
         <v>13.60023579250978</v>
@@ -13626,10 +13626,10 @@
         <v>1.032928706432218</v>
       </c>
       <c r="CZ42" t="n">
-        <v>0.9821967826360616</v>
+        <v>0.9821967826360612</v>
       </c>
       <c r="DA42" t="n">
-        <v>0.9992322314944626</v>
+        <v>0.9992322314944628</v>
       </c>
       <c r="DB42" t="inlineStr">
         <is>
@@ -14186,7 +14186,7 @@
         <v>9.724999999999994</v>
       </c>
       <c r="BX44" t="n">
-        <v>8.658321476792</v>
+        <v>8.658321476792004</v>
       </c>
       <c r="BY44" t="n">
         <v>8.69279915227564</v>

</xml_diff>